<commit_message>
Update default data for gen packages.
</commit_message>
<xml_diff>
--- a/conf/gen/default.xlsx
+++ b/conf/gen/default.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="23715" windowHeight="10305" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="23715" windowHeight="10305"/>
   </bookViews>
   <sheets>
-    <sheet name="emi" sheetId="1" r:id="rId1"/>
+    <sheet name="source" sheetId="1" r:id="rId1"/>
     <sheet name="grid" sheetId="5" r:id="rId2"/>
     <sheet name="year" sheetId="4" r:id="rId3"/>
   </sheets>
@@ -18,10 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="54">
   <si>
-    <t>SOURCES</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>LAT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -228,6 +224,10 @@
   </si>
   <si>
     <t>M4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOURCE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -599,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.15"/>
@@ -616,30 +616,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2">
         <v>180</v>
@@ -648,18 +648,18 @@
         <v>360</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2">
         <v>180</v>
@@ -668,18 +668,18 @@
         <v>360</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="C4" s="2">
         <v>180</v>
@@ -688,10 +688,10 @@
         <v>360</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
@@ -720,7 +720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+    <sheetView topLeftCell="A104" workbookViewId="0">
       <selection activeCell="E104" sqref="E104:E127"/>
     </sheetView>
   </sheetViews>
@@ -733,33 +733,33 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" s="2">
         <v>0.5</v>
@@ -767,16 +767,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3" s="2">
         <v>0.5</v>
@@ -784,16 +784,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" s="2">
         <v>0.5</v>
@@ -801,16 +801,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="2">
         <v>0.5</v>
@@ -818,16 +818,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="2">
         <v>0.5</v>
@@ -835,16 +835,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="2">
         <v>0.5</v>
@@ -852,16 +852,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="2">
         <v>0.5</v>
@@ -869,16 +869,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" s="2">
         <v>0.5</v>
@@ -886,16 +886,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" s="2">
         <v>0.5</v>
@@ -903,16 +903,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="2">
         <v>0.5</v>
@@ -920,16 +920,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" s="2">
         <v>0.5</v>
@@ -937,16 +937,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" s="2">
         <v>0.5</v>
@@ -954,16 +954,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14" s="2">
         <v>0.5</v>
@@ -971,16 +971,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E15" s="2">
         <v>0.5</v>
@@ -988,16 +988,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E16" s="2">
         <v>0.5</v>
@@ -1005,16 +1005,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E17" s="2">
         <v>0.5</v>
@@ -1022,16 +1022,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E18" s="2">
         <v>0.5</v>
@@ -1039,16 +1039,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E19" s="2">
         <v>0.5</v>
@@ -1056,16 +1056,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D20" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E20" s="2">
         <v>0.5</v>
@@ -1073,16 +1073,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E21" s="2">
         <v>0.5</v>
@@ -1090,16 +1090,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E22" s="2">
         <v>0.5</v>
@@ -1107,16 +1107,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E23" s="2">
         <v>0.5</v>
@@ -1124,16 +1124,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E24" s="2">
         <v>0.5</v>
@@ -1141,16 +1141,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E25" s="2">
         <v>0.5</v>
@@ -1158,16 +1158,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E26" s="2">
         <v>0.5</v>
@@ -1175,16 +1175,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E27" s="2">
         <v>0.5</v>
@@ -1192,16 +1192,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E28" s="2">
         <v>0.5</v>
@@ -1209,16 +1209,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D29" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E29" s="2">
         <v>0.5</v>
@@ -1226,16 +1226,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E30" s="2">
         <v>0.5</v>
@@ -1243,16 +1243,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E31" s="2">
         <v>0.5</v>
@@ -1260,16 +1260,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E32" s="2">
         <v>0.5</v>
@@ -1277,16 +1277,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E33" s="2">
         <v>0.5</v>
@@ -1294,16 +1294,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E34" s="2">
         <v>0.5</v>
@@ -1311,16 +1311,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E35" s="2">
         <v>0.5</v>
@@ -1328,16 +1328,16 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E36" s="2">
         <v>0.5</v>
@@ -1345,16 +1345,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E37" s="2">
         <v>0.5</v>
@@ -1362,16 +1362,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D38" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E38" s="2">
         <v>0.5</v>
@@ -1379,16 +1379,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E39" s="2">
         <v>0.5</v>
@@ -1396,16 +1396,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E40" s="2">
         <v>0.5</v>
@@ -1413,16 +1413,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E41" s="2">
         <v>0.5</v>
@@ -1430,16 +1430,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E42" s="2">
         <v>0.5</v>
@@ -1447,16 +1447,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E43" s="2">
         <v>0.5</v>
@@ -1464,16 +1464,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E44" s="2">
         <v>0.5</v>
@@ -1481,16 +1481,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E45" s="2">
         <v>0.5</v>
@@ -1498,16 +1498,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E46" s="2">
         <v>0.5</v>
@@ -1515,16 +1515,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D47" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E47" s="2">
         <v>0.5</v>
@@ -1532,16 +1532,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E48" s="2">
         <v>0.5</v>
@@ -1549,16 +1549,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E49" s="2">
         <v>0.5</v>
@@ -1566,16 +1566,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E50" s="2">
         <v>0.5</v>
@@ -1583,16 +1583,16 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E51" s="2">
         <v>0.5</v>
@@ -1600,16 +1600,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E52" s="2">
         <v>0.5</v>
@@ -1617,16 +1617,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E53" s="2">
         <v>0.5</v>
@@ -1634,16 +1634,16 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E54" s="2">
         <v>0.5</v>
@@ -1651,16 +1651,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E55" s="2">
         <v>0.5</v>
@@ -1668,16 +1668,16 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="D56" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E56" s="2">
         <v>1.5</v>
@@ -1685,16 +1685,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E57" s="2">
         <v>1.5</v>
@@ -1702,16 +1702,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E58" s="2">
         <v>1.5</v>
@@ -1719,16 +1719,16 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E59" s="2">
         <v>1.5</v>
@@ -1736,16 +1736,16 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E60" s="2">
         <v>1.5</v>
@@ -1753,16 +1753,16 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E61" s="2">
         <v>1.5</v>
@@ -1770,16 +1770,16 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E62" s="2">
         <v>1.5</v>
@@ -1787,16 +1787,16 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E63" s="2">
         <v>1.5</v>
@@ -1804,16 +1804,16 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="D64" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E64" s="2">
         <v>1.5</v>
@@ -1821,16 +1821,16 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E65" s="2">
         <v>1.5</v>
@@ -1838,16 +1838,16 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E66" s="2">
         <v>1.5</v>
@@ -1855,16 +1855,16 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E67" s="2">
         <v>1.5</v>
@@ -1872,16 +1872,16 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E68" s="2">
         <v>1.5</v>
@@ -1889,16 +1889,16 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E69" s="2">
         <v>1.5</v>
@@ -1906,16 +1906,16 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E70" s="2">
         <v>1.5</v>
@@ -1923,16 +1923,16 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E71" s="2">
         <v>1.5</v>
@@ -1940,16 +1940,16 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="D72" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E72" s="2">
         <v>1.5</v>
@@ -1957,16 +1957,16 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E73" s="2">
         <v>1.5</v>
@@ -1974,16 +1974,16 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E74" s="2">
         <v>1.5</v>
@@ -1991,16 +1991,16 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E75" s="2">
         <v>1.5</v>
@@ -2008,16 +2008,16 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E76" s="2">
         <v>1.5</v>
@@ -2025,16 +2025,16 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A77" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E77" s="2">
         <v>1.5</v>
@@ -2042,16 +2042,16 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A78" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E78" s="2">
         <v>1.5</v>
@@ -2059,16 +2059,16 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E79" s="2">
         <v>1.5</v>
@@ -2076,16 +2076,16 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A80" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B80" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="D80" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E80" s="2">
         <v>1.5</v>
@@ -2093,16 +2093,16 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E81" s="2">
         <v>1.5</v>
@@ -2110,16 +2110,16 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E82" s="2">
         <v>1.5</v>
@@ -2127,16 +2127,16 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E83" s="2">
         <v>1.5</v>
@@ -2144,16 +2144,16 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A84" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E84" s="2">
         <v>1.5</v>
@@ -2161,16 +2161,16 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A85" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E85" s="2">
         <v>1.5</v>
@@ -2178,16 +2178,16 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E86" s="2">
         <v>1.5</v>
@@ -2195,16 +2195,16 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A87" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E87" s="2">
         <v>1.5</v>
@@ -2212,16 +2212,16 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A88" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C88" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="D88" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E88" s="2">
         <v>1.5</v>
@@ -2229,16 +2229,16 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A89" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C89" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B89" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="D89" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E89" s="2">
         <v>1.5</v>
@@ -2246,16 +2246,16 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A90" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E90" s="2">
         <v>1.5</v>
@@ -2263,16 +2263,16 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A91" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E91" s="2">
         <v>1.5</v>
@@ -2280,16 +2280,16 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A92" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E92" s="2">
         <v>1.5</v>
@@ -2297,16 +2297,16 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A93" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E93" s="2">
         <v>1.5</v>
@@ -2314,16 +2314,16 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A94" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E94" s="2">
         <v>1.5</v>
@@ -2331,16 +2331,16 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A95" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E95" s="2">
         <v>1.5</v>
@@ -2348,16 +2348,16 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A96" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E96" s="2">
         <v>1.5</v>
@@ -2365,16 +2365,16 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A97" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E97" s="2">
         <v>1.5</v>
@@ -2382,16 +2382,16 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A98" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E98" s="2">
         <v>1.5</v>
@@ -2399,16 +2399,16 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A99" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E99" s="2">
         <v>1.5</v>
@@ -2416,16 +2416,16 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A100" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E100" s="2">
         <v>1.5</v>
@@ -2433,16 +2433,16 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A101" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E101" s="2">
         <v>1.5</v>
@@ -2450,16 +2450,16 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A102" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E102" s="2">
         <v>1.5</v>
@@ -2467,16 +2467,16 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A103" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E103" s="2">
         <v>1.5</v>
@@ -2484,16 +2484,16 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A104" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C104" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B104" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="D104" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E104" s="2">
         <v>0.25</v>
@@ -2501,16 +2501,16 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A105" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E105" s="2">
         <v>0.25</v>
@@ -2518,16 +2518,16 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A106" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E106" s="2">
         <v>0.25</v>
@@ -2535,16 +2535,16 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A107" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E107" s="2">
         <v>0.25</v>
@@ -2552,16 +2552,16 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A108" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C108" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B108" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="D108" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E108" s="2">
         <v>0.25</v>
@@ -2569,16 +2569,16 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A109" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E109" s="2">
         <v>0.25</v>
@@ -2586,16 +2586,16 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A110" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E110" s="2">
         <v>0.25</v>
@@ -2603,16 +2603,16 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A111" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E111" s="2">
         <v>0.25</v>
@@ -2620,16 +2620,16 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A112" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C112" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B112" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="D112" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E112" s="2">
         <v>0.25</v>
@@ -2637,16 +2637,16 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A113" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E113" s="2">
         <v>0.25</v>
@@ -2654,16 +2654,16 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A114" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E114" s="2">
         <v>0.25</v>
@@ -2671,16 +2671,16 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A115" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E115" s="2">
         <v>0.25</v>
@@ -2688,16 +2688,16 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A116" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C116" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B116" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="D116" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E116" s="2">
         <v>0.25</v>
@@ -2705,16 +2705,16 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A117" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E117" s="2">
         <v>0.25</v>
@@ -2722,16 +2722,16 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A118" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E118" s="2">
         <v>0.25</v>
@@ -2739,16 +2739,16 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A119" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E119" s="2">
         <v>0.25</v>
@@ -2756,16 +2756,16 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A120" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C120" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B120" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="D120" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E120" s="2">
         <v>0.25</v>
@@ -2773,16 +2773,16 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A121" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C121" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B121" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="D121" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E121" s="2">
         <v>0.25</v>
@@ -2790,16 +2790,16 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A122" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E122" s="2">
         <v>0.25</v>
@@ -2807,16 +2807,16 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A123" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E123" s="2">
         <v>0.25</v>
@@ -2824,16 +2824,16 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A124" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E124" s="2">
         <v>0.25</v>
@@ -2841,16 +2841,16 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A125" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E125" s="2">
         <v>0.25</v>
@@ -2858,16 +2858,16 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A126" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E126" s="2">
         <v>0.25</v>
@@ -2875,16 +2875,16 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A127" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E127" s="2">
         <v>0.25</v>
@@ -2920,13 +2920,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Update config data for GenDataSet0
</commit_message>
<xml_diff>
--- a/conf/gen/default.xlsx
+++ b/conf/gen/default.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="57">
   <si>
     <t>LAT</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -74,14 +74,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;cf.up.root&gt;/&lt;es.name&gt;/EMEP_CO_SOx_NH3_NOx_NMVOC_&lt;es.year&gt;_0.5x0.5.nc|||&lt;es.species&gt;_&lt;es.sector&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;cf.up.root&gt;/&lt;es.name&gt;/&lt;es.species&gt;/v42_&lt;es.species&gt;_&lt;es.year&gt;_IPCC_&lt;es.sector&gt;.0.1x0.1.nc|||emi_&lt;es.speciesLower&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>&lt;cf.up.root&gt;/&lt;es.name&gt;/&lt;es.year&gt;/MEIC-&lt;es.month&gt;.nc|||&lt;es.species&gt;_&lt;es.sector&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -228,6 +220,26 @@
   </si>
   <si>
     <t>SOURCE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>YEAR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;cf.up.root&gt;/&lt;es.name&gt;/&lt;es.species&gt;/v42_&lt;es.species&gt;_&lt;es.year&gt;_IPCC_&lt;es.sector&gt;.nc|||emi_&lt;es.speciesLower&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;cf.up.root&gt;/&lt;es.name&gt;/EMEP_CO_SOx_NH3_NOx_NMVOC_&lt;es.year&gt;.nc|||&lt;es.species&gt;_&lt;es.sector&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -280,7 +292,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -293,8 +305,14 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -599,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.15"/>
@@ -616,7 +634,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>13</v>
@@ -651,7 +669,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
@@ -671,7 +689,7 @@
         <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
@@ -691,7 +709,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
@@ -720,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E127"/>
   <sheetViews>
-    <sheetView topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="E104" sqref="E104:E127"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.15"/>
@@ -733,33 +751,33 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E2" s="2">
         <v>0.5</v>
@@ -767,16 +785,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E3" s="2">
         <v>0.5</v>
@@ -784,16 +802,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E4" s="2">
         <v>0.5</v>
@@ -801,16 +819,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E5" s="2">
         <v>0.5</v>
@@ -818,16 +836,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E6" s="2">
         <v>0.5</v>
@@ -835,16 +853,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E7" s="2">
         <v>0.5</v>
@@ -852,16 +870,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E8" s="2">
         <v>0.5</v>
@@ -869,16 +887,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E9" s="2">
         <v>0.5</v>
@@ -886,16 +904,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E10" s="2">
         <v>0.5</v>
@@ -903,16 +921,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E11" s="2">
         <v>0.5</v>
@@ -920,16 +938,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E12" s="2">
         <v>0.5</v>
@@ -937,16 +955,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E13" s="2">
         <v>0.5</v>
@@ -954,16 +972,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E14" s="2">
         <v>0.5</v>
@@ -971,16 +989,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E15" s="2">
         <v>0.5</v>
@@ -988,16 +1006,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E16" s="2">
         <v>0.5</v>
@@ -1005,16 +1023,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E17" s="2">
         <v>0.5</v>
@@ -1022,16 +1040,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E18" s="2">
         <v>0.5</v>
@@ -1039,16 +1057,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E19" s="2">
         <v>0.5</v>
@@ -1056,16 +1074,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E20" s="2">
         <v>0.5</v>
@@ -1073,16 +1091,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E21" s="2">
         <v>0.5</v>
@@ -1090,16 +1108,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E22" s="2">
         <v>0.5</v>
@@ -1107,16 +1125,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E23" s="2">
         <v>0.5</v>
@@ -1124,16 +1142,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E24" s="2">
         <v>0.5</v>
@@ -1141,16 +1159,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E25" s="2">
         <v>0.5</v>
@@ -1158,16 +1176,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E26" s="2">
         <v>0.5</v>
@@ -1175,16 +1193,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E27" s="2">
         <v>0.5</v>
@@ -1192,16 +1210,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E28" s="2">
         <v>0.5</v>
@@ -1209,16 +1227,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E29" s="2">
         <v>0.5</v>
@@ -1226,16 +1244,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E30" s="2">
         <v>0.5</v>
@@ -1243,16 +1261,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E31" s="2">
         <v>0.5</v>
@@ -1260,16 +1278,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E32" s="2">
         <v>0.5</v>
@@ -1277,16 +1295,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D33" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E33" s="2">
         <v>0.5</v>
@@ -1294,16 +1312,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E34" s="2">
         <v>0.5</v>
@@ -1311,16 +1329,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E35" s="2">
         <v>0.5</v>
@@ -1328,16 +1346,16 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E36" s="2">
         <v>0.5</v>
@@ -1345,16 +1363,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E37" s="2">
         <v>0.5</v>
@@ -1362,16 +1380,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E38" s="2">
         <v>0.5</v>
@@ -1379,16 +1397,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E39" s="2">
         <v>0.5</v>
@@ -1396,16 +1414,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E40" s="2">
         <v>0.5</v>
@@ -1413,16 +1431,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E41" s="2">
         <v>0.5</v>
@@ -1430,16 +1448,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D42" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E42" s="2">
         <v>0.5</v>
@@ -1447,16 +1465,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E43" s="2">
         <v>0.5</v>
@@ -1464,16 +1482,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E44" s="2">
         <v>0.5</v>
@@ -1481,16 +1499,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E45" s="2">
         <v>0.5</v>
@@ -1498,16 +1516,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E46" s="2">
         <v>0.5</v>
@@ -1515,16 +1533,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E47" s="2">
         <v>0.5</v>
@@ -1532,16 +1550,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E48" s="2">
         <v>0.5</v>
@@ -1549,16 +1567,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E49" s="2">
         <v>0.5</v>
@@ -1566,16 +1584,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E50" s="2">
         <v>0.5</v>
@@ -1583,16 +1601,16 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D51" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E51" s="2">
         <v>0.5</v>
@@ -1600,16 +1618,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E52" s="2">
         <v>0.5</v>
@@ -1617,16 +1635,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E53" s="2">
         <v>0.5</v>
@@ -1634,16 +1652,16 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E54" s="2">
         <v>0.5</v>
@@ -1651,16 +1669,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E55" s="2">
         <v>0.5</v>
@@ -1668,16 +1686,16 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E56" s="2">
         <v>1.5</v>
@@ -1685,16 +1703,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="D57" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E57" s="2">
         <v>1.5</v>
@@ -1702,16 +1720,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E58" s="2">
         <v>1.5</v>
@@ -1719,16 +1737,16 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E59" s="2">
         <v>1.5</v>
@@ -1736,16 +1754,16 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E60" s="2">
         <v>1.5</v>
@@ -1753,16 +1771,16 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E61" s="2">
         <v>1.5</v>
@@ -1770,16 +1788,16 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E62" s="2">
         <v>1.5</v>
@@ -1787,16 +1805,16 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E63" s="2">
         <v>1.5</v>
@@ -1804,16 +1822,16 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E64" s="2">
         <v>1.5</v>
@@ -1821,16 +1839,16 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="D65" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E65" s="2">
         <v>1.5</v>
@@ -1838,16 +1856,16 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E66" s="2">
         <v>1.5</v>
@@ -1855,16 +1873,16 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E67" s="2">
         <v>1.5</v>
@@ -1872,16 +1890,16 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E68" s="2">
         <v>1.5</v>
@@ -1889,16 +1907,16 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E69" s="2">
         <v>1.5</v>
@@ -1906,16 +1924,16 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E70" s="2">
         <v>1.5</v>
@@ -1923,16 +1941,16 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E71" s="2">
         <v>1.5</v>
@@ -1940,16 +1958,16 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B72" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="D72" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E72" s="2">
         <v>1.5</v>
@@ -1957,16 +1975,16 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="D73" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E73" s="2">
         <v>1.5</v>
@@ -1974,16 +1992,16 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E74" s="2">
         <v>1.5</v>
@@ -1991,16 +2009,16 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E75" s="2">
         <v>1.5</v>
@@ -2008,16 +2026,16 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E76" s="2">
         <v>1.5</v>
@@ -2025,16 +2043,16 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A77" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E77" s="2">
         <v>1.5</v>
@@ -2042,16 +2060,16 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A78" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E78" s="2">
         <v>1.5</v>
@@ -2059,16 +2077,16 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E79" s="2">
         <v>1.5</v>
@@ -2076,16 +2094,16 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A80" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E80" s="2">
         <v>1.5</v>
@@ -2093,16 +2111,16 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C81" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="D81" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E81" s="2">
         <v>1.5</v>
@@ -2110,16 +2128,16 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E82" s="2">
         <v>1.5</v>
@@ -2127,16 +2145,16 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E83" s="2">
         <v>1.5</v>
@@ -2144,16 +2162,16 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A84" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E84" s="2">
         <v>1.5</v>
@@ -2161,16 +2179,16 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A85" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E85" s="2">
         <v>1.5</v>
@@ -2178,16 +2196,16 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E86" s="2">
         <v>1.5</v>
@@ -2195,16 +2213,16 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A87" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E87" s="2">
         <v>1.5</v>
@@ -2212,16 +2230,16 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A88" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E88" s="2">
         <v>1.5</v>
@@ -2229,16 +2247,16 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A89" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C89" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B89" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="D89" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E89" s="2">
         <v>1.5</v>
@@ -2246,16 +2264,16 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A90" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E90" s="2">
         <v>1.5</v>
@@ -2263,16 +2281,16 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A91" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E91" s="2">
         <v>1.5</v>
@@ -2280,16 +2298,16 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A92" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E92" s="2">
         <v>1.5</v>
@@ -2297,16 +2315,16 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A93" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E93" s="2">
         <v>1.5</v>
@@ -2314,16 +2332,16 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A94" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E94" s="2">
         <v>1.5</v>
@@ -2331,16 +2349,16 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A95" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E95" s="2">
         <v>1.5</v>
@@ -2348,16 +2366,16 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A96" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E96" s="2">
         <v>1.5</v>
@@ -2365,16 +2383,16 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A97" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B97" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="D97" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E97" s="2">
         <v>1.5</v>
@@ -2382,16 +2400,16 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A98" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E98" s="2">
         <v>1.5</v>
@@ -2399,16 +2417,16 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A99" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E99" s="2">
         <v>1.5</v>
@@ -2416,16 +2434,16 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A100" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E100" s="2">
         <v>1.5</v>
@@ -2433,16 +2451,16 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A101" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E101" s="2">
         <v>1.5</v>
@@ -2450,16 +2468,16 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A102" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E102" s="2">
         <v>1.5</v>
@@ -2467,16 +2485,16 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A103" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E103" s="2">
         <v>1.5</v>
@@ -2484,16 +2502,16 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A104" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E104" s="2">
         <v>0.25</v>
@@ -2501,16 +2519,16 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A105" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C105" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B105" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="D105" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E105" s="2">
         <v>0.25</v>
@@ -2518,16 +2536,16 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A106" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E106" s="2">
         <v>0.25</v>
@@ -2535,16 +2553,16 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A107" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E107" s="2">
         <v>0.25</v>
@@ -2552,16 +2570,16 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A108" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B108" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C108" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C108" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="D108" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E108" s="2">
         <v>0.25</v>
@@ -2569,16 +2587,16 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A109" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C109" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B109" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="D109" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E109" s="2">
         <v>0.25</v>
@@ -2586,16 +2604,16 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A110" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E110" s="2">
         <v>0.25</v>
@@ -2603,16 +2621,16 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A111" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E111" s="2">
         <v>0.25</v>
@@ -2620,16 +2638,16 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A112" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E112" s="2">
         <v>0.25</v>
@@ -2637,16 +2655,16 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A113" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C113" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B113" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="D113" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E113" s="2">
         <v>0.25</v>
@@ -2654,16 +2672,16 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A114" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E114" s="2">
         <v>0.25</v>
@@ -2671,16 +2689,16 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A115" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E115" s="2">
         <v>0.25</v>
@@ -2688,16 +2706,16 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A116" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E116" s="2">
         <v>0.25</v>
@@ -2705,16 +2723,16 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A117" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C117" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B117" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="D117" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E117" s="2">
         <v>0.25</v>
@@ -2722,16 +2740,16 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A118" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E118" s="2">
         <v>0.25</v>
@@ -2739,16 +2757,16 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A119" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E119" s="2">
         <v>0.25</v>
@@ -2756,16 +2774,16 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A120" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E120" s="2">
         <v>0.25</v>
@@ -2773,16 +2791,16 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A121" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C121" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B121" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="D121" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E121" s="2">
         <v>0.25</v>
@@ -2790,16 +2808,16 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A122" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E122" s="2">
         <v>0.25</v>
@@ -2807,16 +2825,16 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A123" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E123" s="2">
         <v>0.25</v>
@@ -2824,16 +2842,16 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A124" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E124" s="2">
         <v>0.25</v>
@@ -2841,16 +2859,16 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A125" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C125" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B125" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="D125" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E125" s="2">
         <v>0.25</v>
@@ -2858,16 +2876,16 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A126" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E126" s="2">
         <v>0.25</v>
@@ -2875,26 +2893,26 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A127" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E127" s="2">
         <v>0.25</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:E164">
-    <sortCondition ref="A2:A164"/>
-    <sortCondition ref="B2:B164"/>
-    <sortCondition ref="C2:C164"/>
+  <sortState ref="A2:E127">
+    <sortCondition ref="A2:A127"/>
+    <sortCondition ref="B2:B127"/>
+    <sortCondition ref="C2:C127"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2906,489 +2924,493 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:B29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.75" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="1"/>
-    <col min="3" max="3" width="10.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="10.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="5"/>
+    <col min="3" max="3" width="10.875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="5"/>
+    <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="A1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="4">
+      <c r="A2" s="6">
         <v>1980</v>
       </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="B2" s="5">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="4">
+      <c r="A3" s="6">
         <v>1981</v>
       </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="4">
+      <c r="A4" s="6">
         <v>1982</v>
       </c>
-      <c r="B4" s="1">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="4">
+      <c r="A5" s="6">
         <v>1983</v>
       </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="B5" s="5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="4">
+      <c r="A6" s="6">
         <v>1984</v>
       </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="4">
+      <c r="A7" s="6">
         <v>1985</v>
       </c>
-      <c r="B7" s="1">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1">
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="4">
+      <c r="A8" s="6">
         <v>1986</v>
       </c>
-      <c r="B8" s="1">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="B8" s="5">
+        <v>0</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="4">
+      <c r="A9" s="6">
         <v>1987</v>
       </c>
-      <c r="B9" s="1">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1">
+      <c r="B9" s="5">
+        <v>0</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" s="4">
+      <c r="A10" s="6">
         <v>1988</v>
       </c>
-      <c r="B10" s="1">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1">
+      <c r="B10" s="5">
+        <v>0</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11" s="4">
+      <c r="A11" s="6">
         <v>1989</v>
       </c>
-      <c r="B11" s="1">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1">
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="4">
+      <c r="A12" s="6">
         <v>1990</v>
       </c>
-      <c r="B12" s="1">
-        <v>0</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1">
+      <c r="B12" s="5">
+        <v>0</v>
+      </c>
+      <c r="C12" s="5">
+        <v>1</v>
+      </c>
+      <c r="D12" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="4">
+      <c r="A13" s="6">
         <v>1991</v>
       </c>
-      <c r="B13" s="1">
-        <v>0</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1">
+      <c r="B13" s="5">
+        <v>0</v>
+      </c>
+      <c r="C13" s="5">
+        <v>1</v>
+      </c>
+      <c r="D13" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="4">
+      <c r="A14" s="6">
         <v>1992</v>
       </c>
-      <c r="B14" s="1">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1">
+      <c r="B14" s="5">
+        <v>0</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1</v>
+      </c>
+      <c r="D14" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="4">
+      <c r="A15" s="6">
         <v>1993</v>
       </c>
-      <c r="B15" s="1">
-        <v>0</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1">
+      <c r="B15" s="5">
+        <v>0</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1</v>
+      </c>
+      <c r="D15" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="4">
+      <c r="A16" s="6">
         <v>1994</v>
       </c>
-      <c r="B16" s="1">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1">
+      <c r="B16" s="5">
+        <v>0</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1</v>
+      </c>
+      <c r="D16" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="4">
+      <c r="A17" s="6">
         <v>1995</v>
       </c>
-      <c r="B17" s="1">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1">
+      <c r="B17" s="5">
+        <v>0</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1</v>
+      </c>
+      <c r="D17" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="4">
+      <c r="A18" s="6">
         <v>1996</v>
       </c>
-      <c r="B18" s="1">
-        <v>0</v>
-      </c>
-      <c r="C18" s="1">
-        <v>1</v>
-      </c>
-      <c r="D18" s="1">
+      <c r="B18" s="5">
+        <v>0</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1</v>
+      </c>
+      <c r="D18" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="4">
+      <c r="A19" s="6">
         <v>1997</v>
       </c>
-      <c r="B19" s="1">
-        <v>0</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1">
+      <c r="B19" s="5">
+        <v>0</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1</v>
+      </c>
+      <c r="D19" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="4">
+      <c r="A20" s="6">
         <v>1998</v>
       </c>
-      <c r="B20" s="1">
-        <v>0</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1</v>
-      </c>
-      <c r="D20" s="1">
+      <c r="B20" s="5">
+        <v>0</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1</v>
+      </c>
+      <c r="D20" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="4">
+      <c r="A21" s="6">
         <v>1999</v>
       </c>
-      <c r="B21" s="1">
-        <v>0</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1">
+      <c r="B21" s="5">
+        <v>0</v>
+      </c>
+      <c r="C21" s="5">
+        <v>1</v>
+      </c>
+      <c r="D21" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="4">
+      <c r="A22" s="6">
         <v>2000</v>
       </c>
-      <c r="B22" s="1">
-        <v>0</v>
-      </c>
-      <c r="C22" s="1">
-        <v>1</v>
-      </c>
-      <c r="D22" s="1">
+      <c r="B22" s="5">
+        <v>0</v>
+      </c>
+      <c r="C22" s="5">
+        <v>1</v>
+      </c>
+      <c r="D22" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="4">
+      <c r="A23" s="6">
         <v>2001</v>
       </c>
-      <c r="B23" s="1">
-        <v>0</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1</v>
-      </c>
-      <c r="D23" s="1">
+      <c r="B23" s="5">
+        <v>0</v>
+      </c>
+      <c r="C23" s="5">
+        <v>1</v>
+      </c>
+      <c r="D23" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="4">
+      <c r="A24" s="6">
         <v>2002</v>
       </c>
-      <c r="B24" s="1">
-        <v>0</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1</v>
-      </c>
-      <c r="D24" s="1">
+      <c r="B24" s="5">
+        <v>0</v>
+      </c>
+      <c r="C24" s="5">
+        <v>1</v>
+      </c>
+      <c r="D24" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="4">
+      <c r="A25" s="6">
         <v>2003</v>
       </c>
-      <c r="B25" s="1">
-        <v>0</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-      <c r="D25" s="1">
+      <c r="B25" s="5">
+        <v>0</v>
+      </c>
+      <c r="C25" s="5">
+        <v>1</v>
+      </c>
+      <c r="D25" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="4">
+      <c r="A26" s="6">
         <v>2004</v>
       </c>
-      <c r="B26" s="1">
-        <v>1</v>
-      </c>
-      <c r="C26" s="1">
-        <v>1</v>
-      </c>
-      <c r="D26" s="1">
+      <c r="B26" s="5">
+        <v>1</v>
+      </c>
+      <c r="C26" s="5">
+        <v>1</v>
+      </c>
+      <c r="D26" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="4">
+      <c r="A27" s="6">
         <v>2005</v>
       </c>
-      <c r="B27" s="1">
-        <v>1</v>
-      </c>
-      <c r="C27" s="1">
-        <v>1</v>
-      </c>
-      <c r="D27" s="1">
+      <c r="B27" s="5">
+        <v>1</v>
+      </c>
+      <c r="C27" s="5">
+        <v>1</v>
+      </c>
+      <c r="D27" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="4">
+      <c r="A28" s="6">
         <v>2006</v>
       </c>
-      <c r="B28" s="1">
-        <v>1</v>
-      </c>
-      <c r="C28" s="1">
-        <v>1</v>
-      </c>
-      <c r="D28" s="1">
+      <c r="B28" s="5">
+        <v>1</v>
+      </c>
+      <c r="C28" s="5">
+        <v>1</v>
+      </c>
+      <c r="D28" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="4">
+      <c r="A29" s="6">
         <v>2007</v>
       </c>
-      <c r="B29" s="1">
-        <v>1</v>
-      </c>
-      <c r="C29" s="1">
-        <v>1</v>
-      </c>
-      <c r="D29" s="1">
+      <c r="B29" s="5">
+        <v>1</v>
+      </c>
+      <c r="C29" s="5">
+        <v>1</v>
+      </c>
+      <c r="D29" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="4">
+      <c r="A30" s="6">
         <v>2008</v>
       </c>
-      <c r="B30" s="1">
-        <v>0</v>
-      </c>
-      <c r="C30" s="1">
-        <v>1</v>
-      </c>
-      <c r="D30" s="1">
+      <c r="B30" s="5">
+        <v>0</v>
+      </c>
+      <c r="C30" s="5">
+        <v>1</v>
+      </c>
+      <c r="D30" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="4">
+      <c r="A31" s="6">
         <v>2009</v>
       </c>
-      <c r="B31" s="1">
-        <v>0</v>
-      </c>
-      <c r="C31" s="1">
-        <v>1</v>
-      </c>
-      <c r="D31" s="1">
+      <c r="B31" s="5">
+        <v>0</v>
+      </c>
+      <c r="C31" s="5">
+        <v>1</v>
+      </c>
+      <c r="D31" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A32" s="4">
+      <c r="A32" s="6">
         <v>2010</v>
       </c>
-      <c r="B32" s="1">
-        <v>0</v>
-      </c>
-      <c r="C32" s="1">
-        <v>1</v>
-      </c>
-      <c r="D32" s="1">
+      <c r="B32" s="5">
+        <v>0</v>
+      </c>
+      <c r="C32" s="5">
+        <v>1</v>
+      </c>
+      <c r="D32" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A33" s="4"/>
+      <c r="A33" s="6"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A34" s="4"/>
+      <c r="A34" s="6"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A35" s="4"/>
+      <c r="A35" s="6"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A36" s="4"/>
+      <c r="A36" s="6"/>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A37" s="4"/>
+      <c r="A37" s="6"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A38" s="4"/>
+      <c r="A38" s="6"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A39" s="4"/>
+      <c r="A39" s="6"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A40" s="4"/>
+      <c r="A40" s="6"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A41" s="4"/>
+      <c r="A41" s="6"/>
     </row>
   </sheetData>
   <sortState ref="A2:A7">

</xml_diff>